<commit_message>
0.1.2 translated boss roles
387
</commit_message>
<xml_diff>
--- a/tradept/Excel/Localization/english/R人物列表_Roles_Boss_hotfix.xlsx
+++ b/tradept/Excel/Localization/english/R人物列表_Roles_Boss_hotfix.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xargs01\Downloads\trasl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="f:\Users\isyuricunha\Documents\GitHub\sands-of-salzaar-game-translation\tradept\Excel\Localization\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA619AF-B40C-4A3F-8F60-350C722735AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4AA12E-6F9B-4E55-BDAF-EC4C67C4712E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-300" yWindow="255" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -111,9 +111,6 @@
     <t>魔狼</t>
   </si>
   <si>
-    <t>Canis</t>
-  </si>
-  <si>
     <t>BOSS暗之双星妹</t>
   </si>
   <si>
@@ -335,9 +332,6 @@
     <t>火焰主宰</t>
   </si>
   <si>
-    <t>Lava Sheikh</t>
-  </si>
-  <si>
     <t>dg_skill:T火球术,1</t>
   </si>
   <si>
@@ -399,9 +393,6 @@
   </si>
   <si>
     <t>潮汐恶灵</t>
-  </si>
-  <si>
-    <t>Malignaz</t>
   </si>
   <si>
     <t>dg_skill:冰刃飞梭T,1</t>
@@ -483,9 +474,6 @@
     <t>雄鹰之主</t>
   </si>
   <si>
-    <t>Nasir Sultan</t>
-  </si>
-  <si>
     <t>dg_skill:BOSS翅膀挥击,1</t>
   </si>
   <si>
@@ -606,9 +594,6 @@
     <t>赫斐托斯</t>
   </si>
   <si>
-    <t>Haures</t>
-  </si>
-  <si>
     <t>BOSS火之书精灵</t>
   </si>
   <si>
@@ -678,127 +663,142 @@
     <t>wBOSS女武神</t>
   </si>
   <si>
-    <t>Minero</t>
-  </si>
-  <si>
-    <t>Mago</t>
-  </si>
-  <si>
-    <t>Guerrero de la Llama</t>
-  </si>
-  <si>
-    <t>Rey Canis</t>
-  </si>
-  <si>
-    <t>Dama de Twinstar</t>
-  </si>
-  <si>
-    <t>Espadachín de las Dunas</t>
-  </si>
-  <si>
-    <t>Espadachín Heroico</t>
-  </si>
-  <si>
-    <t>Maestro de la espada aspirante</t>
-  </si>
-  <si>
-    <t>Gran Caballero</t>
-  </si>
-  <si>
-    <t>Caballero Divino</t>
-  </si>
-  <si>
-    <t>Belicista</t>
-  </si>
-  <si>
-    <t>Legendario Herrero</t>
-  </si>
-  <si>
-    <t>Maestro de espadas</t>
-  </si>
-  <si>
-    <t>Mago de la tormenta</t>
-  </si>
-  <si>
-    <t>Árbol gigante</t>
-  </si>
-  <si>
-    <t>Ifrit Guerrero de la Guerra</t>
-  </si>
-  <si>
-    <t>Valkiria</t>
-  </si>
-  <si>
-    <t>Bruja de las flores</t>
-  </si>
-  <si>
     <t>Toxófilo</t>
   </si>
   <si>
-    <t>Sellador de espíritus</t>
-  </si>
-  <si>
-    <t>Espíritu de la naturaleza</t>
-  </si>
-  <si>
-    <t>Guerrero Rúnico</t>
-  </si>
-  <si>
-    <t>Mago de lava</t>
-  </si>
-  <si>
-    <t>Guardián de la montaña</t>
-  </si>
-  <si>
-    <t>Serpiente legendaria</t>
-  </si>
-  <si>
     <t>Sacerdote Nefrita</t>
   </si>
   <si>
-    <t>Rey del Vacío</t>
-  </si>
-  <si>
-    <t>Rey de la Guerra</t>
-  </si>
-  <si>
-    <t>Dragón de hielo</t>
-  </si>
-  <si>
-    <t>Antiguo belicista</t>
-  </si>
-  <si>
-    <t>Dragón de fuego</t>
-  </si>
-  <si>
-    <t>Dragón Veneno</t>
-  </si>
-  <si>
     <t>Núcleo Elemental</t>
   </si>
   <si>
-    <t>Arcángel</t>
-  </si>
-  <si>
-    <t>Rey Fénix</t>
-  </si>
-  <si>
-    <t>Maestro de las llamas</t>
-  </si>
-  <si>
-    <t>Alma heroica</t>
-  </si>
-  <si>
-    <t>Tótem de Burla</t>
-  </si>
-  <si>
-    <t>Araña</t>
-  </si>
-  <si>
-    <t>Gran Águila</t>
-  </si>
-  <si>
-    <t>Mago Ifrit</t>
+    <t>Mineiro</t>
+  </si>
+  <si>
+    <t>Mágico</t>
+  </si>
+  <si>
+    <t>Guerreiro da Chama</t>
+  </si>
+  <si>
+    <t>Rei Canis</t>
+  </si>
+  <si>
+    <t>Canino</t>
+  </si>
+  <si>
+    <t>Senhora Twinstar</t>
+  </si>
+  <si>
+    <t>Espadachim das Dunas</t>
+  </si>
+  <si>
+    <t>Espadachim Heroico</t>
+  </si>
+  <si>
+    <t>Aspirante a Mestre Espadachim</t>
+  </si>
+  <si>
+    <t>Grande cavaleiro</t>
+  </si>
+  <si>
+    <t>Cavaleiro Divino</t>
+  </si>
+  <si>
+    <t>Fomentador da guerra</t>
+  </si>
+  <si>
+    <t>Ferreiro Lendário</t>
+  </si>
+  <si>
+    <t>Mestre de espada</t>
+  </si>
+  <si>
+    <t>Feiticeiro da Tempestade</t>
+  </si>
+  <si>
+    <t>Lava Sheik</t>
+  </si>
+  <si>
+    <t>árvore gigante</t>
+  </si>
+  <si>
+    <t>Ifrit Guerreiro da Guerra</t>
+  </si>
+  <si>
+    <t>Valquíria</t>
+  </si>
+  <si>
+    <t>bruxa das flores</t>
+  </si>
+  <si>
+    <t>Maligno</t>
+  </si>
+  <si>
+    <t>Selador Espiritual</t>
+  </si>
+  <si>
+    <t>Espírito da Natureza</t>
+  </si>
+  <si>
+    <t>Guerreiro Rúnico</t>
+  </si>
+  <si>
+    <t>Assistente de Lava</t>
+  </si>
+  <si>
+    <t>guardião da montanha</t>
+  </si>
+  <si>
+    <t>cobra lendária</t>
+  </si>
+  <si>
+    <t>Sultão Nasir</t>
+  </si>
+  <si>
+    <t>Rei do Vazio</t>
+  </si>
+  <si>
+    <t>Rei da guerra</t>
+  </si>
+  <si>
+    <t>Dragão de Gelo</t>
+  </si>
+  <si>
+    <t>Ex-fomentador da guerra</t>
+  </si>
+  <si>
+    <t>Dragão de fogo</t>
+  </si>
+  <si>
+    <t>Dragão Venenoso</t>
+  </si>
+  <si>
+    <t>Arcanjo</t>
+  </si>
+  <si>
+    <t>Rei Fênix</t>
+  </si>
+  <si>
+    <t>Haurés</t>
+  </si>
+  <si>
+    <t>Mestre das Chamas</t>
+  </si>
+  <si>
+    <t>alma heróica</t>
+  </si>
+  <si>
+    <t>Totem de zombaria</t>
+  </si>
+  <si>
+    <t>Aranha</t>
+  </si>
+  <si>
+    <t>Grande Águia</t>
+  </si>
+  <si>
+    <t>Assistente Ifrit</t>
   </si>
 </sst>
 </file>
@@ -888,7 +888,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1187,10 +1187,14 @@
   <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="C2" sqref="C2:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="60">
       <c r="A1" s="1" t="s">
@@ -1223,7 +1227,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -1243,7 +1247,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -1263,7 +1267,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -1283,7 +1287,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
@@ -1303,7 +1307,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
@@ -1323,7 +1327,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>7</v>
@@ -1343,7 +1347,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>215</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
@@ -1357,835 +1361,835 @@
     </row>
     <row r="9" spans="1:7" ht="135">
       <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="120">
       <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>218</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>218</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
-        <v>218</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" t="s">
-        <v>218</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
-        <v>218</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="45">
       <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="C16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="45">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="60">
       <c r="A21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>219</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s">
-        <v>220</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="60">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>219</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C22" t="s">
-        <v>220</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="60">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>219</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C23" t="s">
-        <v>220</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="G23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="60">
       <c r="A24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>219</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C24" t="s">
-        <v>220</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60">
       <c r="A25" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>219</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C25" t="s">
-        <v>220</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30">
       <c r="A26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" t="s">
+        <v>220</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="s">
-        <v>221</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="G26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30">
       <c r="A27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>220</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C27" t="s">
-        <v>221</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="G27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30">
       <c r="A28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>220</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C28" t="s">
-        <v>221</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="G28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30">
       <c r="A29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>220</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C29" t="s">
-        <v>221</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="G29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30">
       <c r="A30" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>220</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C30" t="s">
-        <v>221</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="G30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30">
       <c r="A31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30">
       <c r="A32" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30">
       <c r="A33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30">
       <c r="A34" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30">
       <c r="A35" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="60">
       <c r="A36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="C36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="60">
       <c r="A37" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="60">
       <c r="A38" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="60">
       <c r="A39" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="60">
       <c r="A40" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45">
       <c r="A41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" t="s">
+        <v>223</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C41" t="s">
-        <v>224</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="G41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="45">
       <c r="A42" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>223</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C42" t="s">
-        <v>224</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="G42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45">
       <c r="A43" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" t="s">
+        <v>223</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C43" t="s">
-        <v>224</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="G43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="45">
       <c r="A44" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C44" t="s">
-        <v>224</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="G44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45">
       <c r="A45" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" t="s">
+        <v>223</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C45" t="s">
-        <v>224</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="G45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="45">
       <c r="A46" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" t="s">
+        <v>224</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C46" t="s">
-        <v>225</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="G46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="45">
       <c r="A47" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>224</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C47" t="s">
-        <v>225</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="G47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="45">
       <c r="A48" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
+        <v>224</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C48" t="s">
-        <v>225</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="G48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="45">
       <c r="A49" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" t="s">
+        <v>224</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C49" t="s">
-        <v>225</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="G49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="45">
       <c r="A50" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>224</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C50" t="s">
-        <v>225</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="G50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="45">
       <c r="A51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="C51" t="s">
+        <v>225</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C51" t="s">
-        <v>226</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="G51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="45">
       <c r="A52" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" t="s">
+        <v>225</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" t="s">
-        <v>226</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="G52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="45">
       <c r="A53" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" t="s">
+        <v>225</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" t="s">
-        <v>226</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="G53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45">
       <c r="A54" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" t="s">
+        <v>225</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C54" t="s">
-        <v>226</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="G54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="45">
       <c r="A55" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" t="s">
+        <v>225</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C55" t="s">
-        <v>226</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="G55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="45">
       <c r="A56" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C56" t="s">
+        <v>226</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C56" t="s">
-        <v>99</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="G56" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="45">
       <c r="A57" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>16</v>
@@ -2196,61 +2200,61 @@
     </row>
     <row r="58" spans="1:7" ht="45">
       <c r="A58" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G58" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="45">
       <c r="A59" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G59" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="45">
       <c r="A60" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C60" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="45">
       <c r="A61" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C61" t="s">
         <v>227</v>
@@ -2259,18 +2263,18 @@
         <v>7</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G61" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="45">
       <c r="A62" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C62" t="s">
         <v>228</v>
@@ -2279,18 +2283,18 @@
         <v>7</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="45">
       <c r="A63" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C63" t="s">
         <v>229</v>
@@ -2299,18 +2303,18 @@
         <v>7</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G63" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="60">
       <c r="A64" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C64" t="s">
         <v>230</v>
@@ -2319,58 +2323,58 @@
         <v>7</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G64" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="45">
       <c r="A65" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65" t="s">
+        <v>231</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C65" t="s">
-        <v>121</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="G65" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="30">
       <c r="A66" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C66" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G66" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="45">
       <c r="A67" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C67" t="s">
         <v>232</v>
@@ -2379,18 +2383,18 @@
         <v>7</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G67" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="45">
       <c r="A68" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C68" t="s">
         <v>233</v>
@@ -2399,18 +2403,18 @@
         <v>7</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G68" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="45">
       <c r="A69" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C69" t="s">
         <v>234</v>
@@ -2419,18 +2423,18 @@
         <v>7</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G69" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="60">
       <c r="A70" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C70" t="s">
         <v>235</v>
@@ -2439,18 +2443,18 @@
         <v>7</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G70" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="45">
       <c r="A71" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C71" t="s">
         <v>236</v>
@@ -2459,18 +2463,18 @@
         <v>7</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G71" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="30">
       <c r="A72" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C72" t="s">
         <v>237</v>
@@ -2484,30 +2488,30 @@
     </row>
     <row r="73" spans="1:7" ht="105">
       <c r="A73" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C73" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G73" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="45">
       <c r="A74" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C74" t="s">
         <v>236</v>
@@ -2516,205 +2520,205 @@
         <v>7</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G74" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="45">
       <c r="A75" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C75" t="s">
-        <v>148</v>
+        <v>238</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G75" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="60">
       <c r="A76" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C76" t="s">
         <v>239</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G76" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="60">
       <c r="A77" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C77" t="s">
         <v>240</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G77" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="60">
       <c r="A78" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C78" t="s">
         <v>241</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G78" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="45">
       <c r="A79" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="45">
       <c r="A80" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C80" t="s">
         <v>242</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G80" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="75">
       <c r="A81" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C81" t="s">
         <v>243</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="45">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C82" t="s">
         <v>244</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G82" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="30">
       <c r="A83" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C83" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G83" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="45">
       <c r="A84" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C84" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G84" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="45">
       <c r="A85" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C85" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G85" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="75">
       <c r="A86" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C86" t="s">
         <v>243</v>
@@ -2723,21 +2727,21 @@
         <v>7</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G86" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="30">
       <c r="A87" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C87" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>7</v>
@@ -2748,13 +2752,13 @@
     </row>
     <row r="88" spans="1:7" ht="30">
       <c r="A88" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C88" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>7</v>
@@ -2765,13 +2769,13 @@
     </row>
     <row r="89" spans="1:7" ht="30">
       <c r="A89" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C89" t="s">
-        <v>189</v>
+        <v>247</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>7</v>
@@ -2782,10 +2786,10 @@
     </row>
     <row r="90" spans="1:7" ht="45">
       <c r="A90" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C90" t="s">
         <v>248</v>
@@ -2799,10 +2803,10 @@
     </row>
     <row r="91" spans="1:7" ht="45">
       <c r="A91" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C91" t="s">
         <v>249</v>
@@ -2811,18 +2815,18 @@
         <v>7</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G91" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="60">
       <c r="A92" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C92" t="s">
         <v>250</v>
@@ -2831,38 +2835,38 @@
         <v>7</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G92" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>25</v>
+        <v>215</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G93" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C94" t="s">
         <v>251</v>
@@ -2871,18 +2875,18 @@
         <v>7</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G94" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C95" t="s">
         <v>252</v>
@@ -2891,18 +2895,18 @@
         <v>7</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G95" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C96" t="s">
         <v>243</v>
@@ -2911,15 +2915,15 @@
         <v>7</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G96" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="105">
       <c r="A97" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>12</v>
@@ -2939,10 +2943,10 @@
     </row>
     <row r="98" spans="1:7" ht="45">
       <c r="A98" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C98" t="s">
         <v>232</v>
@@ -2951,38 +2955,38 @@
         <v>7</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G98" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="45">
       <c r="A99" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C99" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G99" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="60">
       <c r="A100" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C100" t="s">
         <v>230</v>
@@ -2991,18 +2995,18 @@
         <v>7</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G100" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="45">
       <c r="A101" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C101" t="s">
         <v>233</v>
@@ -3011,38 +3015,38 @@
         <v>7</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G101" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="45">
       <c r="A102" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C102" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G102" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="45">
       <c r="A103" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C103" t="s">
         <v>229</v>
@@ -3051,10 +3055,10 @@
         <v>7</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G103" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>